<commit_message>
update hall data + plots
</commit_message>
<xml_diff>
--- a/LEM12/Hall/data.xlsx
+++ b/LEM12/Hall/data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LEM12/Hall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11BF41D8-D46B-564F-AB2F-72463A8BDA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9309BE12-5682-8C46-A129-580611D968E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16000" xr2:uid="{5D8C8EBC-CFB7-974B-9B55-D765D5669E82}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{5D8C8EBC-CFB7-974B-9B55-D765D5669E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">dark </t>
   </si>
@@ -51,6 +75,9 @@
   </si>
   <si>
     <t>FUENTE</t>
+  </si>
+  <si>
+    <t>Rh</t>
   </si>
 </sst>
 </file>
@@ -183,6 +210,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.4677504254908499E-3"/>
+                  <c:y val="6.9990516649942089E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$19</c:f>
@@ -583,10 +661,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$19</c:f>
+              <c:f>Sheet1!$I$2:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.48</c:v>
                 </c:pt>
@@ -597,48 +675,45 @@
                   <c:v>1.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.95</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.98</c:v>
+                  <c:v>2.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.48</c:v>
+                  <c:v>3.05</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.05</c:v>
+                  <c:v>3.57</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.57</c:v>
+                  <c:v>3.98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.98</c:v>
+                  <c:v>4.57</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.57</c:v>
+                  <c:v>5.03</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.03</c:v>
+                  <c:v>5.48</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.48</c:v>
+                  <c:v>6.07</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.07</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.5</c:v>
+                  <c:v>6.97</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.97</c:v>
+                  <c:v>7.49</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.49</c:v>
+                  <c:v>8.08</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.08</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>8.4499999999999993</c:v>
                 </c:pt>
               </c:numCache>
@@ -646,10 +721,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$19</c:f>
+              <c:f>Sheet1!$J$2:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>-87</c:v>
                 </c:pt>
@@ -660,48 +735,45 @@
                   <c:v>-300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-363</c:v>
+                  <c:v>-368</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-368</c:v>
+                  <c:v>-448</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-448</c:v>
+                  <c:v>-514</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-514</c:v>
+                  <c:v>-556</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-556</c:v>
+                  <c:v>-590</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-590</c:v>
+                  <c:v>-618</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-618</c:v>
+                  <c:v>-639</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-639</c:v>
+                  <c:v>-652</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-652</c:v>
+                  <c:v>-675</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-675</c:v>
+                  <c:v>-687</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-687</c:v>
+                  <c:v>-703</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-703</c:v>
+                  <c:v>-716</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-716</c:v>
+                  <c:v>-729</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-729</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>-737</c:v>
                 </c:pt>
               </c:numCache>
@@ -979,56 +1051,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.2428920696051029E-2"/>
-                  <c:y val="7.7397472487423791E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-ES"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$Q$14:$Q$31</c:f>
@@ -1349,6 +1371,464 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3136482939632545E-2"/>
+          <c:y val="0.19486111111111112"/>
+          <c:w val="0.87753018372703417"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>bini</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.14374190726159231"/>
+                  <c:y val="1.9104330708661417E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.49</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.5299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>616</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>662</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>673</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>698</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>705</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5EB9-AA49-A6B8-9D8C3CB3C74C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1758991679"/>
+        <c:axId val="1832588399"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1758991679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1832588399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1832588399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1758991679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1469,6 +1949,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2502,6 +3022,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3122,6 +4158,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>410633</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>8467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4233</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD358F0A-60FA-66FB-8419-A67CA87FCE7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3427,468 +4499,972 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5E43E4-2A42-D543-B971-2DA45FFA9029}">
-  <dimension ref="B1:S31"/>
+  <dimension ref="B1:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V11" zoomScale="206" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="P9" zoomScale="191" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>-6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1">
+        <v>-6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>0.53</v>
+      </c>
+      <c r="C2">
+        <v>-89</v>
+      </c>
+      <c r="D2">
+        <f>-C2</f>
+        <v>89</v>
+      </c>
+      <c r="I2">
+        <v>0.48</v>
+      </c>
+      <c r="J2">
+        <v>-87</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3">
+        <v>-188</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D19" si="0">-C3</f>
+        <v>188</v>
+      </c>
+      <c r="I3">
+        <v>0.97</v>
+      </c>
+      <c r="J3">
+        <v>-182</v>
+      </c>
+      <c r="O3">
+        <v>15.3</v>
+      </c>
+      <c r="P3">
+        <v>0.04</v>
+      </c>
+      <c r="R3">
+        <v>0.59</v>
+      </c>
+      <c r="S3">
+        <v>-0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1.46</v>
+      </c>
+      <c r="C4">
+        <v>-250</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="I4">
+        <v>1.61</v>
+      </c>
+      <c r="J4">
+        <v>-300</v>
+      </c>
+      <c r="O4">
+        <v>15.1</v>
+      </c>
+      <c r="R4">
+        <v>1.32</v>
+      </c>
+      <c r="S4">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>2.04</v>
+      </c>
+      <c r="C5">
+        <v>-342</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+      <c r="I5">
+        <v>1.98</v>
+      </c>
+      <c r="J5">
+        <v>-368</v>
+      </c>
+      <c r="R5">
+        <v>1.47</v>
+      </c>
+      <c r="S5">
+        <v>-0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2.57</v>
+      </c>
+      <c r="C6">
+        <v>-415</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>415</v>
+      </c>
+      <c r="I6">
+        <v>2.48</v>
+      </c>
+      <c r="J6">
+        <v>-448</v>
+      </c>
+      <c r="R6">
+        <v>2.21</v>
+      </c>
+      <c r="S6">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>3.08</v>
+      </c>
+      <c r="C7">
+        <v>-469</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>469</v>
+      </c>
+      <c r="I7">
+        <v>3.05</v>
+      </c>
+      <c r="J7">
+        <v>-514</v>
+      </c>
+      <c r="R7">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>3.52</v>
+      </c>
+      <c r="C8">
+        <v>-507</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>507</v>
+      </c>
+      <c r="I8">
+        <v>3.57</v>
+      </c>
+      <c r="J8">
+        <v>-556</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>4.13</v>
+      </c>
+      <c r="C9">
+        <v>-556</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>556</v>
+      </c>
+      <c r="I9">
+        <v>3.98</v>
+      </c>
+      <c r="J9">
+        <v>-590</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>4.5</v>
+      </c>
+      <c r="C10">
+        <v>-571</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>571</v>
+      </c>
+      <c r="I10">
+        <v>4.57</v>
+      </c>
+      <c r="J10">
+        <v>-618</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>5.13</v>
+      </c>
+      <c r="C11">
+        <v>-601</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>601</v>
+      </c>
+      <c r="I11">
+        <v>5.03</v>
+      </c>
+      <c r="J11">
+        <v>-639</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>5.48</v>
+      </c>
+      <c r="C12">
+        <v>-616</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>616</v>
+      </c>
+      <c r="I12">
+        <v>5.48</v>
+      </c>
+      <c r="J12">
+        <v>-652</v>
+      </c>
+      <c r="T12">
+        <f>T13*0.000001</f>
+        <v>-1.8789802071976325E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>-632</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>632</v>
+      </c>
+      <c r="I13">
+        <v>6.07</v>
+      </c>
+      <c r="J13">
+        <v>-675</v>
+      </c>
+      <c r="P13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T13">
+        <f>T14*1000</f>
+        <v>-1.8789802071976325</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>6.49</v>
+      </c>
+      <c r="C14">
+        <v>-640</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+      <c r="I14">
+        <v>6.5</v>
+      </c>
+      <c r="J14">
+        <v>-687</v>
+      </c>
+      <c r="Q14">
+        <v>0.59</v>
+      </c>
+      <c r="R14">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="S14">
+        <v>99.167622699999995</v>
+      </c>
+      <c r="T14" cm="1">
+        <f t="array" ref="T14:U18">LINEST(R14:R31,S14:S31,TRUE,TRUE)</f>
+        <v>-1.8789802071976325E-3</v>
+      </c>
+      <c r="U14">
+        <v>-3.8592668325693191E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>7.04</v>
+      </c>
+      <c r="C15">
+        <v>-662</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>662</v>
+      </c>
+      <c r="I15">
+        <v>6.97</v>
+      </c>
+      <c r="J15">
+        <v>-703</v>
+      </c>
+      <c r="Q15">
+        <v>0.96</v>
+      </c>
+      <c r="R15">
+        <v>-0.39</v>
+      </c>
+      <c r="S15">
+        <v>163.43791913000001</v>
+      </c>
+      <c r="T15">
+        <v>5.472107527043542E-5</v>
+      </c>
+      <c r="U15">
+        <v>3.0093146648948563E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>7.5</v>
+      </c>
+      <c r="C16">
+        <v>-673</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>673</v>
+      </c>
+      <c r="I16">
+        <v>7.49</v>
+      </c>
+      <c r="J16">
+        <v>-716</v>
+      </c>
+      <c r="Q16">
+        <v>1.77</v>
+      </c>
+      <c r="R16">
+        <v>-0.54</v>
+      </c>
+      <c r="S16">
+        <v>300.49533255</v>
+      </c>
+      <c r="T16">
+        <v>0.98661152835546739</v>
+      </c>
+      <c r="U16">
+        <v>4.168414490957105E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>8.16</v>
+      </c>
+      <c r="C17">
+        <v>-690</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>690</v>
+      </c>
+      <c r="I17">
+        <v>8.08</v>
+      </c>
+      <c r="J17">
+        <v>-729</v>
+      </c>
+      <c r="Q17">
+        <v>2.1</v>
+      </c>
+      <c r="R17">
+        <v>-0.64</v>
+      </c>
+      <c r="S17">
+        <v>350.91283045</v>
+      </c>
+      <c r="T17">
+        <v>1179.0579890523859</v>
+      </c>
+      <c r="U17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="C18">
+        <v>-698</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>698</v>
+      </c>
+      <c r="I18">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="J18">
+        <v>-737</v>
+      </c>
+      <c r="Q18">
+        <v>2.7</v>
+      </c>
+      <c r="R18">
+        <v>-0.82</v>
+      </c>
+      <c r="S18">
+        <v>430.31583839000001</v>
+      </c>
+      <c r="T18">
+        <v>2.0486933574549711</v>
+      </c>
+      <c r="U18">
+        <v>2.7801086989473891E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>8.98</v>
+      </c>
+      <c r="C19">
+        <v>-705</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>705</v>
+      </c>
+      <c r="I19">
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <v>-748</v>
+      </c>
+      <c r="Q19">
+        <v>3.04</v>
+      </c>
+      <c r="R19">
+        <v>-0.89</v>
+      </c>
+      <c r="S19">
+        <v>465.31093351999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q20">
+        <v>3.43</v>
+      </c>
+      <c r="R20">
+        <v>-0.96</v>
+      </c>
+      <c r="S20">
+        <v>499.21661773</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q21">
+        <v>4.05</v>
+      </c>
+      <c r="R21">
+        <v>-1.04</v>
+      </c>
+      <c r="S21">
+        <v>551.18900869000004</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q22">
+        <v>4.55</v>
+      </c>
+      <c r="R22">
+        <v>-1.06</v>
+      </c>
+      <c r="S22">
+        <v>573.00624364999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q23">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="R23">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="S23">
+        <v>591.62506432999999</v>
+      </c>
+      <c r="T23">
+        <f>T15*1000</f>
+        <v>5.4721075270435418E-2</v>
+      </c>
+      <c r="U23" t="s">
+        <v>5</v>
+      </c>
+      <c r="V23">
+        <f>15/T12/0.00005</f>
+        <v>-159661075114.47873</v>
+      </c>
+      <c r="W23">
+        <f>V24*SQRT((0.1/15)^2 + (T23/T13)^2)</f>
+        <v>-1.8712177112808454E-13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q24">
+        <v>5.63</v>
+      </c>
+      <c r="R24">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="S24">
+        <v>621.64101702999994</v>
+      </c>
+      <c r="V24">
+        <f>V23^-1</f>
+        <v>-6.2632673573254415E-12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q25">
+        <v>6.12</v>
+      </c>
+      <c r="R25">
+        <v>-1.27</v>
+      </c>
+      <c r="S25">
+        <v>633.82323498000005</v>
+      </c>
+      <c r="T25" t="e" cm="1">
+        <f t="array" ref="T25">LINEST(R14:R31,S32:S49,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q26">
+        <v>6.52</v>
+      </c>
+      <c r="R26">
+        <v>-1.2</v>
+      </c>
+      <c r="S26">
+        <v>640.89414809000004</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q27">
+        <v>7.02</v>
+      </c>
+      <c r="R27">
+        <v>-1.28</v>
+      </c>
+      <c r="S27">
+        <v>661.29397898000002</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q28">
+        <v>7.53</v>
+      </c>
+      <c r="R28">
+        <v>-1.3</v>
+      </c>
+      <c r="S28">
+        <v>673.66455027999996</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q29">
+        <v>8.44</v>
+      </c>
+      <c r="R29">
+        <v>-1.24</v>
+      </c>
+      <c r="S29">
+        <v>696.25923568999997</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q30">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="R30">
+        <v>-1.35</v>
+      </c>
+      <c r="S30">
+        <v>698.18580003</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Q31">
+        <v>9.06</v>
+      </c>
+      <c r="R31">
+        <v>-1.3</v>
+      </c>
+      <c r="S31">
+        <v>705.98339484999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8820C94F-6A3D-2449-94C2-331D54D805D0}">
+  <dimension ref="A2:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>-6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1">
-        <v>-6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.53</v>
+      </c>
       <c r="B2">
-        <v>0.53</v>
-      </c>
-      <c r="C2">
         <v>-89</v>
       </c>
-      <c r="I2">
-        <v>0.48</v>
-      </c>
-      <c r="J2">
-        <v>-87</v>
-      </c>
-      <c r="O2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="B3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C3">
         <v>-188</v>
       </c>
-      <c r="I3">
-        <v>0.97</v>
-      </c>
-      <c r="J3">
-        <v>-182</v>
-      </c>
-      <c r="O3">
-        <v>15.3</v>
-      </c>
-      <c r="P3">
-        <v>0.04</v>
-      </c>
-      <c r="R3">
-        <v>0.59</v>
-      </c>
-      <c r="S3">
-        <v>-0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1.46</v>
+      </c>
       <c r="B4">
-        <v>1.46</v>
-      </c>
-      <c r="C4">
         <v>-250</v>
       </c>
-      <c r="I4">
-        <v>1.61</v>
-      </c>
-      <c r="J4">
-        <v>-300</v>
-      </c>
-      <c r="O4">
-        <v>15.1</v>
-      </c>
-      <c r="R4">
-        <v>1.32</v>
-      </c>
-      <c r="S4">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2.04</v>
+      </c>
       <c r="B5">
-        <v>2.04</v>
-      </c>
-      <c r="C5">
         <v>-342</v>
       </c>
-      <c r="I5">
-        <v>1.95</v>
-      </c>
-      <c r="J5">
-        <v>-363</v>
-      </c>
-      <c r="R5">
-        <v>1.47</v>
-      </c>
-      <c r="S5">
-        <v>-0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2.57</v>
+      </c>
       <c r="B6">
-        <v>2.57</v>
-      </c>
-      <c r="C6">
         <v>-415</v>
       </c>
-      <c r="I6">
-        <v>1.98</v>
-      </c>
-      <c r="J6">
-        <v>-368</v>
-      </c>
-      <c r="R6">
-        <v>2.21</v>
-      </c>
-      <c r="S6">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3.08</v>
+      </c>
       <c r="B7">
-        <v>3.08</v>
-      </c>
-      <c r="C7">
         <v>-469</v>
       </c>
-      <c r="I7">
-        <v>2.48</v>
-      </c>
-      <c r="J7">
-        <v>-448</v>
-      </c>
-      <c r="R7">
-        <v>2.65</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3.52</v>
+      </c>
       <c r="B8">
-        <v>3.52</v>
-      </c>
-      <c r="C8">
         <v>-507</v>
       </c>
-      <c r="I8">
-        <v>3.05</v>
-      </c>
-      <c r="J8">
-        <v>-514</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4.13</v>
+      </c>
       <c r="B9">
-        <v>4.13</v>
-      </c>
-      <c r="C9">
         <v>-556</v>
       </c>
-      <c r="I9">
-        <v>3.57</v>
-      </c>
-      <c r="J9">
-        <v>-556</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>4.5</v>
+      </c>
       <c r="B10">
-        <v>4.5</v>
-      </c>
-      <c r="C10">
         <v>-571</v>
       </c>
-      <c r="I10">
-        <v>3.98</v>
-      </c>
-      <c r="J10">
-        <v>-590</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5.13</v>
+      </c>
       <c r="B11">
-        <v>5.13</v>
-      </c>
-      <c r="C11">
         <v>-601</v>
       </c>
-      <c r="I11">
-        <v>4.57</v>
-      </c>
-      <c r="J11">
-        <v>-618</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5.48</v>
+      </c>
       <c r="B12">
-        <v>5.48</v>
-      </c>
-      <c r="C12">
         <v>-616</v>
       </c>
-      <c r="I12">
-        <v>5.03</v>
-      </c>
-      <c r="J12">
-        <v>-639</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6</v>
+      </c>
       <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13">
         <v>-632</v>
       </c>
-      <c r="I13">
-        <v>5.48</v>
-      </c>
-      <c r="J13">
-        <v>-652</v>
-      </c>
-      <c r="P13">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6.49</v>
+      </c>
       <c r="B14">
-        <v>6.49</v>
-      </c>
-      <c r="C14">
         <v>-640</v>
       </c>
-      <c r="I14">
-        <v>6.07</v>
-      </c>
-      <c r="J14">
-        <v>-675</v>
-      </c>
-      <c r="Q14">
-        <v>0.59</v>
-      </c>
-      <c r="R14">
-        <v>-0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>7.04</v>
+      </c>
       <c r="B15">
-        <v>7.04</v>
-      </c>
-      <c r="C15">
         <v>-662</v>
       </c>
-      <c r="I15">
-        <v>6.5</v>
-      </c>
-      <c r="J15">
-        <v>-687</v>
-      </c>
-      <c r="Q15">
-        <v>0.96</v>
-      </c>
-      <c r="R15">
-        <v>-0.39</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>7.5</v>
+      </c>
       <c r="B16">
-        <v>7.5</v>
-      </c>
-      <c r="C16">
         <v>-673</v>
       </c>
-      <c r="I16">
-        <v>6.97</v>
-      </c>
-      <c r="J16">
-        <v>-703</v>
-      </c>
-      <c r="Q16">
-        <v>1.77</v>
-      </c>
-      <c r="R16">
-        <v>-0.54</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8.16</v>
+      </c>
       <c r="B17">
-        <v>8.16</v>
-      </c>
-      <c r="C17">
         <v>-690</v>
       </c>
-      <c r="I17">
-        <v>7.49</v>
-      </c>
-      <c r="J17">
-        <v>-716</v>
-      </c>
-      <c r="Q17">
-        <v>2.1</v>
-      </c>
-      <c r="R17">
-        <v>-0.64</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8.5299999999999994</v>
+      </c>
       <c r="B18">
-        <v>8.5299999999999994</v>
-      </c>
-      <c r="C18">
         <v>-698</v>
       </c>
-      <c r="I18">
-        <v>8.08</v>
-      </c>
-      <c r="J18">
-        <v>-729</v>
-      </c>
-      <c r="Q18">
-        <v>2.7</v>
-      </c>
-      <c r="R18">
-        <v>-0.82</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>8.98</v>
+      </c>
       <c r="B19">
-        <v>8.98</v>
-      </c>
-      <c r="C19">
         <v>-705</v>
-      </c>
-      <c r="I19">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="J19">
-        <v>-737</v>
-      </c>
-      <c r="Q19">
-        <v>3.04</v>
-      </c>
-      <c r="R19">
-        <v>-0.89</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="I20">
-        <v>9</v>
-      </c>
-      <c r="J20">
-        <v>-748</v>
-      </c>
-      <c r="Q20">
-        <v>3.43</v>
-      </c>
-      <c r="R20">
-        <v>-0.96</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q21">
-        <v>4.05</v>
-      </c>
-      <c r="R21">
-        <v>-1.04</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q22">
-        <v>4.55</v>
-      </c>
-      <c r="R22">
-        <v>-1.06</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q23">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="R23">
-        <v>-1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q24">
-        <v>5.63</v>
-      </c>
-      <c r="R24">
-        <v>-1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q25">
-        <v>6.12</v>
-      </c>
-      <c r="R25">
-        <v>-1.27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q26">
-        <v>6.52</v>
-      </c>
-      <c r="R26">
-        <v>-1.2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q27">
-        <v>7.02</v>
-      </c>
-      <c r="R27">
-        <v>-1.28</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q28">
-        <v>7.53</v>
-      </c>
-      <c r="R28">
-        <v>-1.3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q29">
-        <v>8.44</v>
-      </c>
-      <c r="R29">
-        <v>-1.24</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q30">
-        <v>8.5399999999999991</v>
-      </c>
-      <c r="R30">
-        <v>-1.35</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q31">
-        <v>9.06</v>
-      </c>
-      <c r="R31">
-        <v>-1.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89639B21-158E-BF47-8663-C12656D8CEA5}">
+  <dimension ref="A2:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.59</v>
+      </c>
+      <c r="B2">
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.96</v>
+      </c>
+      <c r="B3">
+        <v>-0.39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1.77</v>
+      </c>
+      <c r="B4">
+        <v>-0.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2.1</v>
+      </c>
+      <c r="B5">
+        <v>-0.64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2.7</v>
+      </c>
+      <c r="B6">
+        <v>-0.82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3.04</v>
+      </c>
+      <c r="B7">
+        <v>-0.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3.43</v>
+      </c>
+      <c r="B8">
+        <v>-0.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4.05</v>
+      </c>
+      <c r="B9">
+        <v>-1.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>4.55</v>
+      </c>
+      <c r="B10">
+        <v>-1.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="B11">
+        <v>-1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5.63</v>
+      </c>
+      <c r="B12">
+        <v>-1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6.12</v>
+      </c>
+      <c r="B13">
+        <v>-1.27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6.52</v>
+      </c>
+      <c r="B14">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>7.02</v>
+      </c>
+      <c r="B15">
+        <v>-1.28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>7.53</v>
+      </c>
+      <c r="B16">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8.44</v>
+      </c>
+      <c r="B17">
+        <v>-1.24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="B18">
+        <v>-1.35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>9.06</v>
+      </c>
+      <c r="B19">
+        <v>-1.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>